<commit_message>
Mapping en commentaar Astrid
</commit_message>
<xml_diff>
--- a/maps/Coverage-Payer.xlsx
+++ b/maps/Coverage-Payer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/jacob_engel_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{C7E22464-8063-5A48-8AF8-B8CBF9685F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D0516D6-9026-4617-82B6-0F89FAB75936}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{C7E22464-8063-5A48-8AF8-B8CBF9685F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{674A7769-FD95-014E-A9B6-69901756C32F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{4D4295CA-5E27-D54A-800A-CCB7595BF199}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="20220" windowHeight="16780" xr2:uid="{4D4295CA-5E27-D54A-800A-CCB7595BF199}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>xtehr</t>
   </si>
@@ -176,12 +176,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -516,19 +522,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81200B0-CEC8-5048-84D0-94AD3B33B9B6}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.296875" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,187 +542,188 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" t="s">
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>